<commit_message>
Removed wrong cell borders
</commit_message>
<xml_diff>
--- a/Dan/DataTypes.xlsx
+++ b/Dan/DataTypes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aissa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\Summer Research\Drasil\Dan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8B50320-562C-4C1D-A09D-E50ABDED82D6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56685966-0EE3-4841-B3B0-D0AAAA61413D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -445,12 +445,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1113,71 +1113,71 @@
   <dimension ref="A1:AF33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W33" sqref="W33"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="5.44140625" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.53125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.53125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="5.46484375" customWidth="1"/>
+    <col min="5" max="5" width="8.46484375" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" customWidth="1"/>
-    <col min="9" max="9" width="5.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.53125" customWidth="1"/>
+    <col min="8" max="8" width="6.53125" customWidth="1"/>
+    <col min="9" max="9" width="5.46484375" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
-    <col min="11" max="11" width="6.5546875" customWidth="1"/>
+    <col min="11" max="11" width="6.53125" customWidth="1"/>
     <col min="12" max="12" width="9" customWidth="1"/>
-    <col min="13" max="14" width="8.5546875" customWidth="1"/>
-    <col min="15" max="15" width="8.44140625" customWidth="1"/>
-    <col min="16" max="16" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5546875" customWidth="1"/>
-    <col min="18" max="18" width="9.5546875" customWidth="1"/>
+    <col min="13" max="14" width="8.53125" customWidth="1"/>
+    <col min="15" max="15" width="8.46484375" customWidth="1"/>
+    <col min="16" max="16" width="4.86328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.53125" customWidth="1"/>
+    <col min="18" max="18" width="9.53125" customWidth="1"/>
     <col min="19" max="19" width="8.33203125" customWidth="1"/>
-    <col min="20" max="20" width="6.5546875" customWidth="1"/>
-    <col min="21" max="21" width="14.44140625" customWidth="1"/>
+    <col min="20" max="20" width="6.53125" customWidth="1"/>
+    <col min="21" max="21" width="14.46484375" customWidth="1"/>
     <col min="22" max="22" width="6.6640625" customWidth="1"/>
-    <col min="23" max="23" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.1328125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="23.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="20.46484375" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="24.33203125" customWidth="1"/>
     <col min="30" max="30" width="17.6640625" customWidth="1"/>
     <col min="31" max="31" width="12.6640625" customWidth="1"/>
-    <col min="32" max="32" width="26.44140625" customWidth="1"/>
+    <col min="32" max="32" width="26.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.45">
       <c r="C1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="15"/>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="13"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1247,19 +1247,19 @@
       <c r="W2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="12" t="s">
+      <c r="X2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="13"/>
-      <c r="AC2" s="13"/>
-      <c r="AD2" s="13"/>
-      <c r="AE2" s="13"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="15"/>
       <c r="AF2" s="5"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1340,8 +1340,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A6" s="10" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1378,8 +1378,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A7" s="10"/>
       <c r="B7" s="8" t="s">
         <v>36</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1444,8 +1444,8 @@
       </c>
       <c r="W8" s="3"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A9" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1461,15 +1461,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A10" s="10"/>
       <c r="B10" s="8" t="s">
         <v>101</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G10" t="s">
@@ -1478,7 +1478,7 @@
       <c r="I10" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="P10" s="6" t="s">
@@ -1491,8 +1491,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A11" s="10"/>
       <c r="B11" s="8" t="s">
         <v>45</v>
       </c>
@@ -1508,7 +1508,7 @@
       <c r="I11" t="s">
         <v>20</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="3" t="s">
         <v>20</v>
       </c>
       <c r="N11" t="s">
@@ -1524,8 +1524,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A12" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1537,7 +1537,7 @@
       <c r="H12" t="s">
         <v>20</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="3" t="s">
         <v>20</v>
       </c>
       <c r="L12" t="s">
@@ -1562,8 +1562,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A13" s="10"/>
       <c r="B13" s="8" t="s">
         <v>50</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="6"/>
-      <c r="K13" t="s">
+      <c r="K13" s="3" t="s">
         <v>20</v>
       </c>
       <c r="L13" t="s">
@@ -1608,7 +1608,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="6"/>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="3" t="s">
         <v>20</v>
       </c>
       <c r="M14" t="s">
@@ -1650,7 +1650,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1663,7 +1663,7 @@
       <c r="J15" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="3" t="s">
         <v>20</v>
       </c>
       <c r="M15" t="s">
@@ -1688,7 +1688,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1710,7 +1710,7 @@
       <c r="J16" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="N16" t="s">
@@ -1726,7 +1726,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -1799,8 +1799,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A19" s="10" t="s">
         <v>68</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -1822,8 +1822,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A20" s="14"/>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A20" s="10"/>
       <c r="B20" s="8" t="s">
         <v>70</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -1983,7 +1983,7 @@
       </c>
       <c r="Z25" s="6"/>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B27" s="8" t="s">
         <v>86</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B29" s="8" t="s">
         <v>89</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>90</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>92</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>96</v>
       </c>

</xml_diff>

<commit_message>
Updated class diagram (#784)
* Arrow going to Unit now faces the right way

* Removed wrong cell borders

* Removed Symbol Form

* Made may-have arrow dashed

* Updated Class Diagram as per issue #704
</commit_message>
<xml_diff>
--- a/Dan/DataTypes.xlsx
+++ b/Dan/DataTypes.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\aissa\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samcr\Desktop\Summer Research\Drasil\Dan\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C8B50320-562C-4C1D-A09D-E50ABDED82D6}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56685966-0EE3-4841-B3B0-D0AAAA61413D}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9072" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="9075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -445,12 +445,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1113,71 +1113,71 @@
   <dimension ref="A1:AF33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="W33" sqref="W33"/>
+      <selection activeCell="L20" sqref="L20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="20.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.5546875" style="8" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="7.5546875" style="2" customWidth="1"/>
-    <col min="4" max="4" width="5.44140625" customWidth="1"/>
-    <col min="5" max="5" width="8.44140625" customWidth="1"/>
+    <col min="1" max="1" width="20.1328125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.53125" style="8" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="7.53125" style="2" customWidth="1"/>
+    <col min="4" max="4" width="5.46484375" customWidth="1"/>
+    <col min="5" max="5" width="8.46484375" customWidth="1"/>
     <col min="6" max="6" width="8.33203125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.5546875" customWidth="1"/>
-    <col min="8" max="8" width="6.5546875" customWidth="1"/>
-    <col min="9" max="9" width="5.44140625" customWidth="1"/>
+    <col min="7" max="7" width="11.53125" customWidth="1"/>
+    <col min="8" max="8" width="6.53125" customWidth="1"/>
+    <col min="9" max="9" width="5.46484375" customWidth="1"/>
     <col min="10" max="10" width="9" customWidth="1"/>
-    <col min="11" max="11" width="6.5546875" customWidth="1"/>
+    <col min="11" max="11" width="6.53125" customWidth="1"/>
     <col min="12" max="12" width="9" customWidth="1"/>
-    <col min="13" max="14" width="8.5546875" customWidth="1"/>
-    <col min="15" max="15" width="8.44140625" customWidth="1"/>
-    <col min="16" max="16" width="4.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.5546875" customWidth="1"/>
-    <col min="18" max="18" width="9.5546875" customWidth="1"/>
+    <col min="13" max="14" width="8.53125" customWidth="1"/>
+    <col min="15" max="15" width="8.46484375" customWidth="1"/>
+    <col min="16" max="16" width="4.86328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.53125" customWidth="1"/>
+    <col min="18" max="18" width="9.53125" customWidth="1"/>
     <col min="19" max="19" width="8.33203125" customWidth="1"/>
-    <col min="20" max="20" width="6.5546875" customWidth="1"/>
-    <col min="21" max="21" width="14.44140625" customWidth="1"/>
+    <col min="20" max="20" width="6.53125" customWidth="1"/>
+    <col min="21" max="21" width="14.46484375" customWidth="1"/>
     <col min="22" max="22" width="6.6640625" customWidth="1"/>
-    <col min="23" max="23" width="3.109375" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="3.1328125" bestFit="1" customWidth="1"/>
     <col min="24" max="24" width="23.6640625" style="2" bestFit="1" customWidth="1"/>
     <col min="25" max="25" width="24.33203125" bestFit="1" customWidth="1"/>
-    <col min="26" max="27" width="20.44140625" bestFit="1" customWidth="1"/>
+    <col min="26" max="27" width="20.46484375" bestFit="1" customWidth="1"/>
     <col min="28" max="28" width="14.6640625" bestFit="1" customWidth="1"/>
     <col min="29" max="29" width="24.33203125" customWidth="1"/>
     <col min="30" max="30" width="17.6640625" customWidth="1"/>
     <col min="31" max="31" width="12.6640625" customWidth="1"/>
-    <col min="32" max="32" width="26.44140625" customWidth="1"/>
+    <col min="32" max="32" width="26.46484375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.45">
       <c r="C1" s="1" t="s">
         <v>103</v>
       </c>
-      <c r="D1" s="10" t="s">
+      <c r="D1" s="11" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
-      <c r="G1" s="11"/>
-      <c r="H1" s="11"/>
-      <c r="I1" s="11"/>
-      <c r="J1" s="11"/>
-      <c r="K1" s="11"/>
-      <c r="L1" s="11"/>
-      <c r="M1" s="11"/>
-      <c r="N1" s="11"/>
-      <c r="O1" s="11"/>
-      <c r="P1" s="11"/>
-      <c r="Q1" s="11"/>
-      <c r="R1" s="11"/>
-      <c r="S1" s="11"/>
-      <c r="T1" s="11"/>
-      <c r="U1" s="11"/>
-      <c r="V1" s="11"/>
-      <c r="W1" s="15"/>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
+      <c r="E1" s="12"/>
+      <c r="F1" s="12"/>
+      <c r="G1" s="12"/>
+      <c r="H1" s="12"/>
+      <c r="I1" s="12"/>
+      <c r="J1" s="12"/>
+      <c r="K1" s="12"/>
+      <c r="L1" s="12"/>
+      <c r="M1" s="12"/>
+      <c r="N1" s="12"/>
+      <c r="O1" s="12"/>
+      <c r="P1" s="12"/>
+      <c r="Q1" s="12"/>
+      <c r="R1" s="12"/>
+      <c r="S1" s="12"/>
+      <c r="T1" s="12"/>
+      <c r="U1" s="12"/>
+      <c r="V1" s="12"/>
+      <c r="W1" s="13"/>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A2" s="5" t="s">
         <v>0</v>
       </c>
@@ -1247,19 +1247,19 @@
       <c r="W2" s="5" t="s">
         <v>21</v>
       </c>
-      <c r="X2" s="12" t="s">
+      <c r="X2" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="Y2" s="13"/>
-      <c r="Z2" s="13"/>
-      <c r="AA2" s="13"/>
-      <c r="AB2" s="13"/>
-      <c r="AC2" s="13"/>
-      <c r="AD2" s="13"/>
-      <c r="AE2" s="13"/>
+      <c r="Y2" s="15"/>
+      <c r="Z2" s="15"/>
+      <c r="AA2" s="15"/>
+      <c r="AB2" s="15"/>
+      <c r="AC2" s="15"/>
+      <c r="AD2" s="15"/>
+      <c r="AE2" s="15"/>
       <c r="AF2" s="5"/>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>18</v>
       </c>
@@ -1285,7 +1285,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A4" t="s">
         <v>25</v>
       </c>
@@ -1314,7 +1314,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A5" t="s">
         <v>28</v>
       </c>
@@ -1340,8 +1340,8 @@
         <v>32</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A6" s="14" t="s">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A6" s="10" t="s">
         <v>33</v>
       </c>
       <c r="B6" s="8" t="s">
@@ -1378,8 +1378,8 @@
         <v>37</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A7" s="14"/>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A7" s="10"/>
       <c r="B7" s="8" t="s">
         <v>36</v>
       </c>
@@ -1417,7 +1417,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A8" t="s">
         <v>40</v>
       </c>
@@ -1444,8 +1444,8 @@
       </c>
       <c r="W8" s="3"/>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A9" s="14" t="s">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A9" s="10" t="s">
         <v>43</v>
       </c>
       <c r="B9" s="8" t="s">
@@ -1461,15 +1461,15 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A10" s="14"/>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A10" s="10"/>
       <c r="B10" s="8" t="s">
         <v>101</v>
       </c>
       <c r="C10" s="2" t="s">
         <v>20</v>
       </c>
-      <c r="F10" s="2" t="s">
+      <c r="F10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="G10" t="s">
@@ -1478,7 +1478,7 @@
       <c r="I10" t="s">
         <v>20</v>
       </c>
-      <c r="K10" s="2" t="s">
+      <c r="K10" s="3" t="s">
         <v>20</v>
       </c>
       <c r="P10" s="6" t="s">
@@ -1491,8 +1491,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A11" s="14"/>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A11" s="10"/>
       <c r="B11" s="8" t="s">
         <v>45</v>
       </c>
@@ -1508,7 +1508,7 @@
       <c r="I11" t="s">
         <v>20</v>
       </c>
-      <c r="K11" t="s">
+      <c r="K11" s="3" t="s">
         <v>20</v>
       </c>
       <c r="N11" t="s">
@@ -1524,8 +1524,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A12" s="14" t="s">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A12" s="10" t="s">
         <v>46</v>
       </c>
       <c r="B12" s="8" t="s">
@@ -1537,7 +1537,7 @@
       <c r="H12" t="s">
         <v>20</v>
       </c>
-      <c r="K12" t="s">
+      <c r="K12" s="3" t="s">
         <v>20</v>
       </c>
       <c r="L12" t="s">
@@ -1562,8 +1562,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
-      <c r="A13" s="14"/>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.45">
+      <c r="A13" s="10"/>
       <c r="B13" s="8" t="s">
         <v>50</v>
       </c>
@@ -1583,7 +1583,7 @@
         <v>20</v>
       </c>
       <c r="J13" s="6"/>
-      <c r="K13" t="s">
+      <c r="K13" s="3" t="s">
         <v>20</v>
       </c>
       <c r="L13" t="s">
@@ -1608,7 +1608,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A14" t="s">
         <v>51</v>
       </c>
@@ -1628,7 +1628,7 @@
         <v>20</v>
       </c>
       <c r="J14" s="6"/>
-      <c r="K14" s="2" t="s">
+      <c r="K14" s="3" t="s">
         <v>20</v>
       </c>
       <c r="M14" t="s">
@@ -1650,7 +1650,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A15" t="s">
         <v>53</v>
       </c>
@@ -1663,7 +1663,7 @@
       <c r="J15" t="s">
         <v>20</v>
       </c>
-      <c r="K15" s="2" t="s">
+      <c r="K15" s="3" t="s">
         <v>20</v>
       </c>
       <c r="M15" t="s">
@@ -1688,7 +1688,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.45">
       <c r="A16" t="s">
         <v>55</v>
       </c>
@@ -1710,7 +1710,7 @@
       <c r="J16" t="s">
         <v>20</v>
       </c>
-      <c r="K16" s="2" t="s">
+      <c r="K16" s="3" t="s">
         <v>20</v>
       </c>
       <c r="N16" t="s">
@@ -1726,7 +1726,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="17" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A17" t="s">
         <v>58</v>
       </c>
@@ -1752,7 +1752,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -1799,8 +1799,8 @@
         <v>67</v>
       </c>
     </row>
-    <row r="19" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A19" s="14" t="s">
+    <row r="19" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A19" s="10" t="s">
         <v>68</v>
       </c>
       <c r="B19" s="8" t="s">
@@ -1822,8 +1822,8 @@
         <v>20</v>
       </c>
     </row>
-    <row r="20" spans="1:27" x14ac:dyDescent="0.3">
-      <c r="A20" s="14"/>
+    <row r="20" spans="1:27" x14ac:dyDescent="0.45">
+      <c r="A20" s="10"/>
       <c r="B20" s="8" t="s">
         <v>70</v>
       </c>
@@ -1846,7 +1846,7 @@
         <v>71</v>
       </c>
     </row>
-    <row r="21" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -1872,7 +1872,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="22" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A22" t="s">
         <v>75</v>
       </c>
@@ -1904,7 +1904,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="23" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A23" t="s">
         <v>77</v>
       </c>
@@ -1942,7 +1942,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="24" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A24" t="s">
         <v>79</v>
       </c>
@@ -1971,7 +1971,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="25" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A25" t="s">
         <v>98</v>
       </c>
@@ -1983,7 +1983,7 @@
       </c>
       <c r="Z25" s="6"/>
     </row>
-    <row r="26" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A26" t="s">
         <v>84</v>
       </c>
@@ -2003,7 +2003,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="27" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B27" s="8" t="s">
         <v>86</v>
       </c>
@@ -2032,7 +2032,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A28" t="s">
         <v>87</v>
       </c>
@@ -2082,7 +2082,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="29" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:27" x14ac:dyDescent="0.45">
       <c r="B29" s="8" t="s">
         <v>89</v>
       </c>
@@ -2120,7 +2120,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="30" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A30" t="s">
         <v>90</v>
       </c>
@@ -2161,7 +2161,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="31" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A31" t="s">
         <v>92</v>
       </c>
@@ -2193,7 +2193,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:27" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:27" x14ac:dyDescent="0.45">
       <c r="A32" t="s">
         <v>94</v>
       </c>
@@ -2234,7 +2234,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="33" spans="1:23" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:23" x14ac:dyDescent="0.45">
       <c r="A33" t="s">
         <v>96</v>
       </c>

</xml_diff>